<commit_message>
modified charts. client area now is a df which can be downloaded and added my picture. TO DO: modify the nav price taken for purchase/sale add donut chart for strtegies. build calculator for investment days. add pictures. add to the empty tabs
</commit_message>
<xml_diff>
--- a/returns.xlsx
+++ b/returns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\Education\masters\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE83E23-9FF7-4EC0-9ADD-F7AD8B456DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD35E90-F7E0-483B-8167-5B4C4BC861CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="10440" windowWidth="19410" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="2625" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -53,21 +53,22 @@
     <t>Fund_1</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>NAV BM</t>
   </si>
   <si>
     <t>NAV Fund</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="dd/mm/yy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -100,9 +101,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,7 +387,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,7 +397,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -412,13 +413,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -429,7 +430,7 @@
         <v>-6.1000000000000004E-3</v>
       </c>
       <c r="C2">
-        <v>0.03</v>
+        <v>-1.8730339999999401E-3</v>
       </c>
       <c r="D2">
         <f>B2+1</f>
@@ -437,11 +438,11 @@
       </c>
       <c r="E2">
         <f>1+C2</f>
-        <v>1.03</v>
-      </c>
-      <c r="F2">
+        <v>0.99812696600000006</v>
+      </c>
+      <c r="F2" s="3">
         <f>C2-B2</f>
-        <v>3.61E-2</v>
+        <v>4.2269660000000603E-3</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -458,7 +459,7 @@
         <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C3">
-        <v>0.04</v>
+        <v>-5.8106475404052782E-3</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D50" si="0">B3+1</f>
@@ -466,11 +467,11 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E50" si="1">1+C3</f>
-        <v>1.04</v>
-      </c>
-      <c r="F3">
+        <v>0.99418935245959472</v>
+      </c>
+      <c r="F3" s="3">
         <f t="shared" ref="F3:F50" si="2">C3-B3</f>
-        <v>4.3000000000000003E-2</v>
+        <v>-2.8106475404052781E-3</v>
       </c>
       <c r="G3">
         <f>G2*D2</f>
@@ -478,7 +479,7 @@
       </c>
       <c r="H3">
         <f>H2*E2</f>
-        <v>103</v>
+        <v>99.81269660000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -489,7 +490,7 @@
         <v>8.2000000000000007E-3</v>
       </c>
       <c r="C4">
-        <v>0.03</v>
+        <v>4.424214101106605E-3</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -497,19 +498,19 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>1.03</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
-        <v>2.18E-2</v>
+        <v>1.0044242141011066</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>-3.7757858988933957E-3</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G50" si="3">G3*D3</f>
+        <f>G3*D3</f>
         <v>99.091830000000002</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H50" si="4">H3*E3</f>
-        <v>107.12</v>
+        <f t="shared" ref="G4:H19" si="3">H3*E3</f>
+        <v>99.232720200000003</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -520,7 +521,7 @@
         <v>-5.4000000000000003E-3</v>
       </c>
       <c r="C5">
-        <v>0.02</v>
+        <v>-2.9458217482632998E-3</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -528,19 +529,19 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>1.02</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>2.5399999999999999E-2</v>
+        <v>0.9970541782517367</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>2.4541782517367005E-3</v>
       </c>
       <c r="G5">
         <f t="shared" si="3"/>
         <v>99.904383006000003</v>
       </c>
       <c r="H5">
-        <f t="shared" si="4"/>
-        <v>110.3336</v>
+        <f t="shared" si="3"/>
+        <v>99.671747000000011</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -551,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.01</v>
+        <v>9.1358107015653278E-3</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -559,19 +560,19 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>1.01</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>0.01</v>
+        <v>1.0091358107015653</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>9.1358107015653278E-3</v>
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
         <v>99.364899337767611</v>
       </c>
       <c r="H6">
-        <f t="shared" si="4"/>
-        <v>112.540272</v>
+        <f t="shared" si="3"/>
+        <v>99.37813180000002</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -582,7 +583,7 @@
         <v>3.8E-3</v>
       </c>
       <c r="C7">
-        <v>-6.1000000000000004E-3</v>
+        <v>4.4746889755282737E-3</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -590,19 +591,19 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0.99390000000000001</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>-9.9000000000000008E-3</v>
+        <v>1.0044746889755283</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>6.7468897552827372E-4</v>
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
         <v>99.364899337767611</v>
       </c>
       <c r="H7">
-        <f t="shared" si="4"/>
-        <v>113.66567472</v>
+        <f t="shared" si="3"/>
+        <v>100.28603160000003</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -613,7 +614,7 @@
         <v>-3.8999999999999998E-3</v>
       </c>
       <c r="C8">
-        <v>-3.0000000000000001E-3</v>
+        <v>-5.8920444124975768E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -621,19 +622,19 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>0.997</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>8.9999999999999976E-4</v>
+        <v>0.99410795558750242</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.992044412497577E-3</v>
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
         <v>99.742485955251126</v>
       </c>
       <c r="H8">
-        <f t="shared" si="4"/>
-        <v>112.972314104208</v>
+        <f t="shared" si="3"/>
+        <v>100.73478040000003</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -644,27 +645,27 @@
         <v>-2.9499999999999998E-2</v>
       </c>
       <c r="C9">
-        <v>8.2000000000000007E-3</v>
+        <v>-2.6877530402142913E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
         <v>0.97050000000000003</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
-        <v>1.0082</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>3.7699999999999997E-2</v>
+        <f>1+C9</f>
+        <v>0.97312246959785709</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>2.6224695978570856E-3</v>
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
         <v>99.353490260025652</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
-        <v>112.63339716189537</v>
+        <f t="shared" si="3"/>
+        <v>100.14124660000004</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -675,7 +676,7 @@
         <v>-8.9999999999999998E-4</v>
       </c>
       <c r="C10">
-        <v>-5.4000000000000003E-3</v>
+        <v>-1.9361188943745056E-3</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -683,19 +684,19 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.99460000000000004</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>-4.5000000000000005E-3</v>
+        <v>0.99806388110562549</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.0361188943745056E-3</v>
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
         <v>96.422562297354901</v>
       </c>
       <c r="H10">
-        <f t="shared" si="4"/>
-        <v>113.55699101862291</v>
+        <f t="shared" si="3"/>
+        <v>97.44969720000006</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -706,7 +707,7 @@
         <v>1.09E-2</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.1159699605462592E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -714,19 +715,19 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>-1.09E-2</v>
+        <v>1.0111596996054626</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5969960546259191E-4</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
         <v>96.335781991287277</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
-        <v>112.94378326712236</v>
+        <f t="shared" si="3"/>
+        <v>97.261023000000066</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -737,7 +738,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="C12">
-        <v>3.8E-3</v>
+        <v>5.6617817049149366E-3</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -745,19 +746,19 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>1.0038</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>-3.5000000000000001E-3</v>
+        <v>1.0056617817049149</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.6382182950850635E-3</v>
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
         <v>97.385842014992306</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
-        <v>112.94378326712236</v>
+        <f t="shared" si="3"/>
+        <v>98.34642680000006</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -768,7 +769,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="C13">
-        <v>-3.8999999999999998E-3</v>
+        <v>1.0264344942186421E-2</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -776,19 +777,19 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>0.99609999999999999</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
-        <v>-1.49E-2</v>
+        <v>1.0102643449421864</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>-7.3565505781357857E-4</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
         <v>98.096758661701756</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
-        <v>113.37296964353743</v>
+        <f t="shared" si="3"/>
+        <v>98.903242800000058</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,7 +800,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
       <c r="C14">
-        <v>-2.9499999999999998E-2</v>
+        <v>2.6189405369279051E-3</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -807,19 +808,19 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>0.97050000000000003</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
-        <v>-2.9099999999999997E-2</v>
+        <v>1.0026189405369279</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>3.0189405369279053E-3</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
         <v>99.175823006980465</v>
       </c>
       <c r="H14">
-        <f t="shared" si="4"/>
-        <v>112.93081506192763</v>
+        <f t="shared" si="3"/>
+        <v>99.91841980000008</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -830,7 +831,7 @@
         <v>-1.11E-2</v>
       </c>
       <c r="C15">
-        <v>-8.9999999999999998E-4</v>
+        <v>-8.848288215227873E-3</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -838,19 +839,19 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>0.99909999999999999</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
-        <v>1.0200000000000001E-2</v>
+        <v>0.99115171178477213</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2517117847721275E-3</v>
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
         <v>99.136152677777673</v>
       </c>
       <c r="H15">
-        <f t="shared" si="4"/>
-        <v>109.59935601760077</v>
+        <f t="shared" si="3"/>
+        <v>100.18010020000008</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -861,7 +862,7 @@
         <v>-1.0699999999999999E-2</v>
       </c>
       <c r="C16">
-        <v>1.09E-2</v>
+        <v>-1.0188815868395595E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -869,19 +870,19 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>1.0108999999999999</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
-        <v>2.1600000000000001E-2</v>
+        <v>0.9898111841316044</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>5.1118413160440405E-4</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
         <v>98.035741383054344</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
-        <v>109.50071659718493</v>
+        <f t="shared" si="3"/>
+        <v>99.293677800000069</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -892,7 +893,7 @@
         <v>-4.3E-3</v>
       </c>
       <c r="C17">
-        <v>7.3000000000000001E-3</v>
+        <v>-1.4909547092535336E-3</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -900,19 +901,19 @@
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>1.0073000000000001</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="2"/>
-        <v>1.1599999999999999E-2</v>
+        <v>0.99850904529074647</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>2.8090452907464664E-3</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
         <v>96.986758950255663</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
-        <v>110.69427440809424</v>
+        <f t="shared" si="3"/>
+        <v>98.281992800000069</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -923,7 +924,7 @@
         <v>-2.2000000000000001E-3</v>
       </c>
       <c r="C18">
-        <v>1.0999999999999999E-2</v>
+        <v>-3.779590012983336E-3</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -931,19 +932,19 @@
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>1.0109999999999999</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="2"/>
-        <v>1.32E-2</v>
+        <v>0.99622040998701666</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.5795900129833358E-3</v>
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
         <v>96.569715886769572</v>
       </c>
       <c r="H18">
-        <f t="shared" si="4"/>
-        <v>111.50234261127335</v>
+        <f t="shared" si="3"/>
+        <v>98.13545880000008</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -954,7 +955,7 @@
         <v>1.26E-2</v>
       </c>
       <c r="C19">
-        <v>-4.0000000000000002E-4</v>
+        <v>7.5195766007079001E-3</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -962,19 +963,19 @@
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>0.99960000000000004</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="2"/>
-        <v>-1.2999999999999999E-2</v>
+        <v>1.0075195766007079</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>-5.0804233992921E-3</v>
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
         <v>96.357262511818675</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
-        <v>112.72886837999735</v>
+        <f t="shared" si="3"/>
+        <v>97.764547000000064</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -985,7 +986,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="C20">
-        <v>-1.11E-2</v>
+        <v>3.7200176102067939E-3</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -993,19 +994,19 @@
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>0.9889</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="2"/>
-        <v>-1.66E-2</v>
+        <v>1.0037200176102068</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.7799823897932058E-3</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G20:H35" si="4">G19*D19</f>
         <v>97.57136401946758</v>
       </c>
       <c r="H20">
         <f t="shared" si="4"/>
-        <v>112.68377683264536</v>
+        <v>98.499695000000074</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1016,7 +1017,7 @@
         <v>-1.11E-2</v>
       </c>
       <c r="C21">
-        <v>-1.0699999999999999E-2</v>
+        <v>-8.441632352348738E-3</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -1024,19 +1025,19 @@
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>0.98929999999999996</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
-        <v>4.0000000000000105E-4</v>
+        <v>0.99155836764765126</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>2.6583676476512625E-3</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98.108006521574652</v>
       </c>
       <c r="H21">
         <f t="shared" si="4"/>
-        <v>111.43298690980301</v>
+        <v>98.866115600000072</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1047,7 +1048,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="C22">
-        <v>-4.3E-3</v>
+        <v>5.9183411125629526E-4</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -1055,19 +1056,19 @@
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>0.99570000000000003</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="2"/>
-        <v>-5.8999999999999999E-3</v>
+        <v>1.0005918341112563</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.0081658887437048E-3</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97.01900764918517</v>
       </c>
       <c r="H22">
         <f t="shared" si="4"/>
-        <v>110.2406539498681</v>
+        <v>98.031524200000064</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,7 +1079,7 @@
         <v>-1.54E-2</v>
       </c>
       <c r="C23">
-        <v>-2.2000000000000001E-3</v>
+        <v>-1.232574409007392E-2</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
@@ -1086,19 +1087,19 @@
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>0.99780000000000002</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="2"/>
-        <v>1.32E-2</v>
+        <v>0.98767425590992608</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>3.0742559099260804E-3</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97.174238061423864</v>
       </c>
       <c r="H23">
         <f t="shared" si="4"/>
-        <v>109.76661913788368</v>
+        <v>98.089542600000073</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,7 +1110,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="C24">
-        <v>1.26E-2</v>
+        <v>3.3170033900316032E-3</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -1117,19 +1118,19 @@
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>1.0125999999999999</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="2"/>
-        <v>1.0999999999999999E-2</v>
+        <v>1.0033170033900316</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.7170033900316031E-3</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95.677754795277934</v>
       </c>
       <c r="H24">
         <f t="shared" si="4"/>
-        <v>109.52513257578033</v>
+        <v>96.880516000000071</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1140,7 +1141,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="C25">
-        <v>5.4999999999999997E-3</v>
+        <v>3.69674167479217E-3</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -1148,19 +1149,19 @@
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>1.0055000000000001</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="2"/>
-        <v>4.3999999999999994E-3</v>
+        <v>1.0036967416747922</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5967416747921697E-3</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95.830839202950386</v>
       </c>
       <c r="H25">
         <f t="shared" si="4"/>
-        <v>110.90514924623515</v>
+        <v>97.201869000000087</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1171,7 +1172,7 @@
         <v>1.83E-2</v>
       </c>
       <c r="C26">
-        <v>-1.11E-2</v>
+        <v>1.2855602537530153E-2</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
@@ -1179,19 +1180,19 @@
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>0.9889</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="2"/>
-        <v>-2.9400000000000003E-2</v>
+        <v>1.0128556025375302</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>-5.4443974624698473E-3</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95.936253126073638</v>
       </c>
       <c r="H26">
         <f t="shared" si="4"/>
-        <v>111.51512756708945</v>
+        <v>97.561199200000075</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1202,7 +1203,7 @@
         <v>-2.0999999999999999E-3</v>
       </c>
       <c r="C27">
-        <v>1.6000000000000001E-3</v>
+        <v>-2.8026803496294939E-4</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
@@ -1210,19 +1211,19 @@
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>1.0016</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="2"/>
-        <v>3.7000000000000002E-3</v>
+        <v>0.99971973196503705</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>1.8197319650370505E-3</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97.691886558280785</v>
       </c>
       <c r="H27">
         <f t="shared" si="4"/>
-        <v>110.27730965109475</v>
+        <v>98.815407200000081</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1233,7 +1234,7 @@
         <v>0.01</v>
       </c>
       <c r="C28">
-        <v>-1.54E-2</v>
+        <v>8.1366678149741301E-3</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
@@ -1241,19 +1242,19 @@
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>0.98460000000000003</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
-        <v>-2.5399999999999999E-2</v>
+        <v>1.0081366678149741</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.8633321850258702E-3</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97.486733596508401</v>
       </c>
       <c r="H28">
         <f t="shared" si="4"/>
-        <v>110.45375334653652</v>
+        <v>98.787712400000075</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1264,7 +1265,7 @@
         <v>8.8000000000000005E-3</v>
       </c>
       <c r="C29">
-        <v>1.6000000000000001E-3</v>
+        <v>8.1303632982581142E-3</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
@@ -1272,19 +1273,19 @@
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>1.0016</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="2"/>
-        <v>-7.2000000000000007E-3</v>
+        <v>1.0081303632982581</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.6963670174188632E-4</v>
       </c>
       <c r="G29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98.461600932473488</v>
       </c>
       <c r="H29">
         <f t="shared" si="4"/>
-        <v>108.75276554499986</v>
+        <v>99.591515200000075</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1295,7 +1296,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
       <c r="C30">
-        <v>1.1000000000000001E-3</v>
+        <v>3.8797193863873147E-3</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
@@ -1303,19 +1304,19 @@
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>1.0011000000000001</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="2"/>
-        <v>-5.0000000000000001E-3</v>
+        <v>1.0038797193863873</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.2202806136126857E-3</v>
       </c>
       <c r="G30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99.328063020679252</v>
       </c>
       <c r="H30">
         <f t="shared" si="4"/>
-        <v>108.92676996987187</v>
+        <v>100.40123040000007</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1326,7 +1327,7 @@
         <v>5.3E-3</v>
       </c>
       <c r="C31">
-        <v>1.83E-2</v>
+        <v>3.784622754949174E-3</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
@@ -1334,19 +1335,19 @@
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>1.0183</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="2"/>
-        <v>1.3000000000000001E-2</v>
+        <v>1.0037846227549492</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.515377245050826E-3</v>
       </c>
       <c r="G31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99.933964205105397</v>
       </c>
       <c r="H31">
         <f t="shared" si="4"/>
-        <v>109.04658941683874</v>
+        <v>100.79075900000009</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1357,7 +1358,7 @@
         <v>-2.8999999999999998E-3</v>
       </c>
       <c r="C32">
-        <v>-2.0999999999999999E-3</v>
+        <v>-2.1841372375230872E-4</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
@@ -1365,19 +1366,19 @@
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
-        <v>0.99790000000000001</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="2"/>
-        <v>7.9999999999999993E-4</v>
+        <v>0.99978158627624769</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="2"/>
+        <v>2.6815862762476911E-3</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100.46361421539247</v>
       </c>
       <c r="H32">
         <f t="shared" si="4"/>
-        <v>111.04214200316689</v>
+        <v>101.1722140000001</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1388,7 +1389,7 @@
         <v>-1.46E-2</v>
       </c>
       <c r="C33">
-        <v>0.01</v>
+        <v>-1.6872105118265424E-2</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
@@ -1396,19 +1397,19 @@
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>1.01</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="2"/>
-        <v>2.46E-2</v>
+        <v>0.98312789488173458</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.2721051182654235E-3</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100.17226973416783</v>
       </c>
       <c r="H33">
         <f t="shared" si="4"/>
-        <v>110.80895350496024</v>
+        <v>101.15011660000009</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1419,7 +1420,7 @@
         <v>9.1999999999999998E-3</v>
       </c>
       <c r="C34">
-        <v>8.8000000000000005E-3</v>
+        <v>4.3905071194336731E-3</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
@@ -1427,19 +1428,19 @@
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>1.0087999999999999</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="2"/>
-        <v>-3.9999999999999931E-4</v>
+        <v>1.0043905071194337</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.8094928805663267E-3</v>
       </c>
       <c r="G34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98.709754596048981</v>
       </c>
       <c r="H34">
         <f t="shared" si="4"/>
-        <v>111.91704304000984</v>
+        <v>99.443501200000085</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1450,7 +1451,7 @@
         <v>-4.7000000000000002E-3</v>
       </c>
       <c r="C35">
-        <v>6.1000000000000004E-3</v>
+        <v>-2.3006723082396041E-3</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
@@ -1458,19 +1459,19 @@
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
-        <v>1.0061</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="2"/>
-        <v>1.0800000000000001E-2</v>
+        <v>0.9976993276917604</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="2"/>
+        <v>2.3993276917603961E-3</v>
       </c>
       <c r="G35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99.617884338332644</v>
       </c>
       <c r="H35">
         <f t="shared" si="4"/>
-        <v>112.90191301876192</v>
+        <v>99.880108600000099</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1481,7 +1482,7 @@
         <v>5.3E-3</v>
       </c>
       <c r="C36">
-        <v>5.3E-3</v>
+        <v>3.0419471660245723E-3</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
@@ -1489,19 +1490,19 @@
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>1.0053000000000001</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.0030419471660246</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.2580528339754278E-3</v>
       </c>
       <c r="G36">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G36:H50" si="5">G35*D35</f>
         <v>99.14968028194248</v>
       </c>
       <c r="H36">
-        <f t="shared" si="4"/>
-        <v>113.59061468817636</v>
+        <f t="shared" si="5"/>
+        <v>99.650317200000117</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1512,7 +1513,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C37">
-        <v>-2.8999999999999998E-3</v>
+        <v>-4.6491702724469341E-3</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
@@ -1520,19 +1521,19 @@
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>0.99709999999999999</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="2"/>
-        <v>2.1000000000000003E-3</v>
+        <v>0.99535082972755307</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="2"/>
+        <v>3.5082972755306596E-4</v>
       </c>
       <c r="G37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.675173587436788</v>
       </c>
       <c r="H37">
-        <f t="shared" si="4"/>
-        <v>114.19264494602371</v>
+        <f t="shared" si="5"/>
+        <v>99.953448200000111</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1543,7 +1544,7 @@
         <v>-7.6E-3</v>
       </c>
       <c r="C38">
-        <v>-1.46E-2</v>
+        <v>-8.6030492959989768E-3</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
@@ -1551,19 +1552,19 @@
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>0.98540000000000005</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="2"/>
-        <v>-7.0000000000000001E-3</v>
+        <v>0.99139695070400102</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.0030492959989768E-3</v>
       </c>
       <c r="G38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.176797719499604</v>
       </c>
       <c r="H38">
-        <f t="shared" si="4"/>
-        <v>113.86148627568024</v>
+        <f t="shared" si="5"/>
+        <v>99.48874760000011</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1574,7 +1575,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="C39">
-        <v>9.1999999999999998E-3</v>
+        <v>6.5106408118165149E-3</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
@@ -1582,19 +1583,19 @@
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
-        <v>1.0092000000000001</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="2"/>
-        <v>2E-3</v>
+        <v>1.0065106408118165</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.8935918818348492E-4</v>
       </c>
       <c r="G39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>98.423054056831404</v>
       </c>
       <c r="H39">
-        <f t="shared" si="4"/>
-        <v>112.19910857605531</v>
+        <f t="shared" si="5"/>
+        <v>98.632841000000113</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1605,7 +1606,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="C40">
-        <v>-4.7000000000000002E-3</v>
+        <v>5.7222299381625152E-3</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
@@ -1613,19 +1614,19 @@
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
-        <v>0.99529999999999996</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="2"/>
-        <v>-8.6E-3</v>
+        <v>1.0057222299381625</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="2"/>
+        <v>1.8222299381625154E-3</v>
       </c>
       <c r="G40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.131700046040606</v>
       </c>
       <c r="H40">
-        <f t="shared" si="4"/>
-        <v>113.23134037495502</v>
+        <f t="shared" si="5"/>
+        <v>99.275004000000123</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1636,7 +1637,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="C41">
-        <v>5.3E-3</v>
+        <v>-2.0558540791145719E-3</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
@@ -1644,19 +1645,19 @@
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
-        <v>1.0053000000000001</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="2"/>
-        <v>1.7000000000000001E-3</v>
+        <v>0.99794414592088543</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="2"/>
+        <v>-5.6558540791145718E-3</v>
       </c>
       <c r="G41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.51831367622016</v>
       </c>
       <c r="H41">
-        <f t="shared" si="4"/>
-        <v>112.69915307519273</v>
+        <f t="shared" si="5"/>
+        <v>99.843078400000124</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1667,7 +1668,7 @@
         <v>-9.4999999999999998E-3</v>
       </c>
       <c r="C42">
-        <v>-5.0000000000000001E-3</v>
+        <v>-7.1890315507882052E-3</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
@@ -1675,19 +1676,19 @@
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
-        <v>0.995</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="2"/>
-        <v>4.4999999999999997E-3</v>
+        <v>0.99281096844921179</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="2"/>
+        <v>2.3109684492117945E-3</v>
       </c>
       <c r="G42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.876579605454552</v>
       </c>
       <c r="H42">
-        <f t="shared" si="4"/>
-        <v>113.29645858649126</v>
+        <f t="shared" si="5"/>
+        <v>99.637815600000124</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1698,7 +1699,7 @@
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="C43">
-        <v>-7.6E-3</v>
+        <v>6.2035907209438967E-3</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
@@ -1706,19 +1707,19 @@
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
-        <v>0.99239999999999995</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="2"/>
-        <v>-1.43E-2</v>
+        <v>1.0062035907209439</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.9640927905610348E-4</v>
       </c>
       <c r="G43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>98.927752099202735</v>
       </c>
       <c r="H43">
-        <f t="shared" si="4"/>
-        <v>112.72997629355879</v>
+        <f t="shared" si="5"/>
+        <v>98.921516200000113</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1729,7 +1730,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C44">
-        <v>7.1999999999999998E-3</v>
+        <v>7.0837262362721809E-4</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
@@ -1737,19 +1738,19 @@
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
-        <v>1.0072000000000001</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="2"/>
-        <v>6.8999999999999999E-3</v>
+        <v>1.0007083726236272</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="2"/>
+        <v>4.0837262362721812E-4</v>
       </c>
       <c r="G44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.590568038267392</v>
       </c>
       <c r="H44">
-        <f t="shared" si="4"/>
-        <v>111.87322847372774</v>
+        <f t="shared" si="5"/>
+        <v>99.535184800000138</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1760,7 +1761,7 @@
         <v>-2.7000000000000001E-3</v>
       </c>
       <c r="C45">
-        <v>3.8999999999999998E-3</v>
+        <v>-1.3132341769123146E-3</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
@@ -1768,19 +1769,19 @@
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
-        <v>1.0039</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="2"/>
-        <v>6.6E-3</v>
+        <v>0.99868676582308769</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3867658230876856E-3</v>
       </c>
       <c r="G45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.620445208678873</v>
       </c>
       <c r="H45">
-        <f t="shared" si="4"/>
-        <v>112.67871571873859</v>
+        <f t="shared" si="5"/>
+        <v>99.605692800000128</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1791,7 +1792,7 @@
         <v>1.04E-2</v>
       </c>
       <c r="C46">
-        <v>3.5999999999999999E-3</v>
+        <v>8.7211177053738709E-3</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
@@ -1799,19 +1800,19 @@
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
-        <v>1.0036</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="2"/>
-        <v>-6.7999999999999996E-3</v>
+        <v>1.0087211177053739</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.6788822946261286E-3</v>
       </c>
       <c r="G46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>99.351470006615443</v>
       </c>
       <c r="H46">
-        <f t="shared" si="4"/>
-        <v>113.11816271004167</v>
+        <f t="shared" si="5"/>
+        <v>99.47488720000014</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1822,7 +1823,7 @@
         <v>-1E-4</v>
       </c>
       <c r="C47">
-        <v>-9.4999999999999998E-3</v>
+        <v>-7.0934705805980602E-4</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
@@ -1830,19 +1831,19 @@
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
-        <v>0.99050000000000005</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="2"/>
-        <v>-9.4000000000000004E-3</v>
+        <v>0.99929065294194019</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.0934705805980598E-4</v>
       </c>
       <c r="G47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100.38472529468424</v>
       </c>
       <c r="H47">
-        <f t="shared" si="4"/>
-        <v>113.52538809579782</v>
+        <f t="shared" si="5"/>
+        <v>100.34241940000013</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1853,7 +1854,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="C48">
-        <v>6.7000000000000002E-3</v>
+        <v>5.4592921177925025E-3</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
@@ -1861,19 +1862,19 @@
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
-        <v>1.0066999999999999</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="2"/>
-        <v>4.3E-3</v>
+        <v>1.0054592921177925</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="2"/>
+        <v>3.0592921177925027E-3</v>
       </c>
       <c r="G48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100.37468682215477</v>
       </c>
       <c r="H48">
-        <f t="shared" si="4"/>
-        <v>112.44689690888775</v>
+        <f t="shared" si="5"/>
+        <v>100.27124180000013</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1884,7 +1885,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="C49">
-        <v>2.9999999999999997E-4</v>
+        <v>3.5590993689522676E-3</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
@@ -1892,19 +1893,19 @@
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
-        <v>1.0003</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="2"/>
-        <v>-2.0999999999999999E-3</v>
+        <v>1.0035590993689523</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1590993689522678E-3</v>
       </c>
       <c r="G49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100.61558607052794</v>
       </c>
       <c r="H49">
-        <f t="shared" si="4"/>
-        <v>113.20029111817729</v>
+        <f t="shared" si="5"/>
+        <v>100.81865180000014</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1915,7 +1916,7 @@
         <v>-4.3E-3</v>
       </c>
       <c r="C50">
-        <v>-2.7000000000000001E-3</v>
+        <v>-3.8284410484509257E-3</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
@@ -1923,19 +1924,19 @@
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
-        <v>0.99729999999999996</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="2"/>
-        <v>1.5999999999999999E-3</v>
+        <v>0.99617155895154907</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="2"/>
+        <v>4.715589515490743E-4</v>
       </c>
       <c r="G50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100.8570634770972</v>
       </c>
       <c r="H50">
-        <f t="shared" si="4"/>
-        <v>113.23425120551273</v>
+        <f t="shared" si="5"/>
+        <v>101.17747540000013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit before creatig the calculator
</commit_message>
<xml_diff>
--- a/returns.xlsx
+++ b/returns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\Education\masters\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD35E90-F7E0-483B-8167-5B4C4BC861CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1181B8-C0A4-4364-9CF6-9AA46E378884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="2625" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0481C0C-C6C1-4105-9AF5-89537EAF92D6}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,15 +462,15 @@
         <v>-5.8106475404052782E-3</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D50" si="0">B3+1</f>
+        <f t="shared" ref="D3:D51" si="0">B3+1</f>
         <v>0.997</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E50" si="1">1+C3</f>
+        <f t="shared" ref="E3:E51" si="1">1+C3</f>
         <v>0.99418935245959472</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F50" si="2">C3-B3</f>
+        <f t="shared" ref="F3:F51" si="2">C3-B3</f>
         <v>-2.8106475404052781E-3</v>
       </c>
       <c r="G3">
@@ -1497,7 +1497,7 @@
         <v>-2.2580528339754278E-3</v>
       </c>
       <c r="G36">
-        <f t="shared" ref="G36:H50" si="5">G35*D35</f>
+        <f t="shared" ref="G36:H51" si="5">G35*D35</f>
         <v>99.14968028194248</v>
       </c>
       <c r="H36">
@@ -1937,6 +1937,37 @@
       <c r="H50">
         <f t="shared" si="5"/>
         <v>101.17747540000013</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>45709</v>
+      </c>
+      <c r="B51">
+        <v>-1.7100000000000001E-2</v>
+      </c>
+      <c r="C51">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>0.9829</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000003E-3</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="5"/>
+        <v>100.42337810414568</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="5"/>
+        <v>100.79012340000014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>